<commit_message>
modifying jupyter notebook and xlsx files
</commit_message>
<xml_diff>
--- a/Average.xlsx
+++ b/Average.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -41,6 +41,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -220,10 +221,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -239,7 +240,7 @@
       </c>
       <c r="B2" s="4" t="n">
         <f aca="false">AVERAGE(A2:A9)</f>
-        <v>9</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,7 +250,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>